<commit_message>
re-ran the anonymisation cuz there seemed to be some problems in the original files
</commit_message>
<xml_diff>
--- a/anon_data/anon_data_global2.xlsx
+++ b/anon_data/anon_data_global2.xlsx
@@ -570,7 +570,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -726,7 +726,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B10" t="n">
         <v>1</v>
@@ -804,7 +804,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B13" t="n">
         <v>0</v>
@@ -1142,7 +1142,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B26" t="n">
         <v>0</v>
@@ -1168,7 +1168,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B27" t="n">
         <v>0</v>
@@ -1194,7 +1194,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B28" t="n">
         <v>1</v>
@@ -1428,7 +1428,7 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B37" t="n">
         <v>0</v>
@@ -1480,7 +1480,7 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B39" t="n">
         <v>1</v>
@@ -1766,7 +1766,7 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B50" t="n">
         <v>0</v>
@@ -1792,7 +1792,7 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B51" t="n">
         <v>0</v>
@@ -1844,7 +1844,7 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B53" t="n">
         <v>0</v>
@@ -1974,7 +1974,7 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B58" t="n">
         <v>0</v>
@@ -2026,7 +2026,7 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B60" t="n">
         <v>1</v>
@@ -2078,7 +2078,7 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B62" t="n">
         <v>1</v>
@@ -2104,7 +2104,7 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B63" t="n">
         <v>1</v>
@@ -2312,7 +2312,7 @@
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B71" t="n">
         <v>1</v>
@@ -2338,7 +2338,7 @@
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B72" t="n">
         <v>0</v>
@@ -2494,7 +2494,7 @@
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B78" t="n">
         <v>0</v>
@@ -2546,7 +2546,7 @@
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B80" t="n">
         <v>1</v>
@@ -2572,7 +2572,7 @@
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B81" t="n">
         <v>0</v>
@@ -2598,7 +2598,7 @@
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B82" t="n">
         <v>0</v>
@@ -2806,7 +2806,7 @@
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B90" t="n">
         <v>0</v>
@@ -2858,7 +2858,7 @@
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B92" t="n">
         <v>0</v>
@@ -2910,7 +2910,7 @@
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B94" t="n">
         <v>0</v>
@@ -3118,7 +3118,7 @@
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B102" t="n">
         <v>1</v>
@@ -3196,7 +3196,7 @@
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B105" t="n">
         <v>0</v>
@@ -3274,7 +3274,7 @@
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B108" t="n">
         <v>0</v>
@@ -3352,7 +3352,7 @@
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B111" t="n">
         <v>0</v>
@@ -3456,7 +3456,7 @@
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B115" t="n">
         <v>0</v>
@@ -3508,7 +3508,7 @@
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B117" t="n">
         <v>1</v>
@@ -3586,7 +3586,7 @@
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B120" t="n">
         <v>0</v>
@@ -3612,7 +3612,7 @@
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B121" t="n">
         <v>0</v>
@@ -3794,7 +3794,7 @@
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B128" t="n">
         <v>1</v>
@@ -4080,7 +4080,7 @@
     </row>
     <row r="139">
       <c r="A139" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B139" t="n">
         <v>0</v>
@@ -4236,7 +4236,7 @@
     </row>
     <row r="145">
       <c r="A145" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B145" t="n">
         <v>0</v>
@@ -4314,7 +4314,7 @@
     </row>
     <row r="148">
       <c r="A148" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B148" t="n">
         <v>0</v>
@@ -4626,7 +4626,7 @@
     </row>
     <row r="160">
       <c r="A160" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B160" t="n">
         <v>0</v>
@@ -4678,7 +4678,7 @@
     </row>
     <row r="162">
       <c r="A162" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B162" t="n">
         <v>0</v>
@@ -4756,7 +4756,7 @@
     </row>
     <row r="165">
       <c r="A165" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B165" t="n">
         <v>0</v>
@@ -4990,7 +4990,7 @@
     </row>
     <row r="174">
       <c r="A174" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B174" t="n">
         <v>1</v>
@@ -5068,7 +5068,7 @@
     </row>
     <row r="177">
       <c r="A177" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B177" t="n">
         <v>0</v>
@@ -5094,7 +5094,7 @@
     </row>
     <row r="178">
       <c r="A178" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B178" t="n">
         <v>0</v>
@@ -5198,7 +5198,7 @@
     </row>
     <row r="182">
       <c r="A182" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B182" t="n">
         <v>0</v>
@@ -5276,7 +5276,7 @@
     </row>
     <row r="185">
       <c r="A185" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B185" t="n">
         <v>0</v>
@@ -5458,7 +5458,7 @@
     </row>
     <row r="192">
       <c r="A192" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B192" t="n">
         <v>0</v>
@@ -5536,7 +5536,7 @@
     </row>
     <row r="195">
       <c r="A195" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B195" t="n">
         <v>1</v>
@@ -5614,7 +5614,7 @@
     </row>
     <row r="198">
       <c r="A198" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B198" t="n">
         <v>0</v>

</xml_diff>